<commit_message>
Adjust passenger rail and freight aircraft costs
</commit_message>
<xml_diff>
--- a/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
+++ b/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\trans\AVMC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-minnesota\InputData\trans\AVMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF646FD-413E-4B0A-A984-B8BBA1CEB9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="405" windowWidth="24435" windowHeight="16275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -448,7 +447,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="9">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -1274,7 +1273,7 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1309,149 +1308,150 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="140" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="141">
-    <cellStyle name="20% - Accent1 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Calculation 2" xfId="40" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Check Cell 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Comma 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Comma 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Comma 2 2 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Comma 2 2 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Comma 2 3" xfId="45" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Comma 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Comma 4" xfId="47" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Comma 5" xfId="48" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Comma 6" xfId="49" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Comma 7" xfId="50" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Currency 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Currency 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Currency 3 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Data" xfId="54" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Data no deci" xfId="55" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Data Superscript" xfId="56" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="57" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Good 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Heading 1 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Heading 2 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Heading 3 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Heading 4 2" xfId="63" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Hed Side" xfId="13" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Hed Side bold" xfId="64" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Hed Side Indent" xfId="65" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="66" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Hed Top" xfId="68" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="15"/>
+    <cellStyle name="20% - Accent2 2" xfId="16"/>
+    <cellStyle name="20% - Accent3 2" xfId="17"/>
+    <cellStyle name="20% - Accent4 2" xfId="18"/>
+    <cellStyle name="20% - Accent5 2" xfId="19"/>
+    <cellStyle name="20% - Accent6 2" xfId="20"/>
+    <cellStyle name="40% - Accent1 2" xfId="21"/>
+    <cellStyle name="40% - Accent2 2" xfId="22"/>
+    <cellStyle name="40% - Accent3 2" xfId="23"/>
+    <cellStyle name="40% - Accent4 2" xfId="24"/>
+    <cellStyle name="40% - Accent5 2" xfId="25"/>
+    <cellStyle name="40% - Accent6 2" xfId="26"/>
+    <cellStyle name="60% - Accent1 2" xfId="27"/>
+    <cellStyle name="60% - Accent2 2" xfId="28"/>
+    <cellStyle name="60% - Accent3 2" xfId="29"/>
+    <cellStyle name="60% - Accent4 2" xfId="30"/>
+    <cellStyle name="60% - Accent5 2" xfId="31"/>
+    <cellStyle name="60% - Accent6 2" xfId="32"/>
+    <cellStyle name="Accent1 2" xfId="33"/>
+    <cellStyle name="Accent2 2" xfId="34"/>
+    <cellStyle name="Accent3 2" xfId="35"/>
+    <cellStyle name="Accent4 2" xfId="36"/>
+    <cellStyle name="Accent5 2" xfId="37"/>
+    <cellStyle name="Accent6 2" xfId="38"/>
+    <cellStyle name="Bad 2" xfId="39"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Calculation 2" xfId="40"/>
+    <cellStyle name="Check Cell 2" xfId="41"/>
+    <cellStyle name="Comma 2" xfId="42"/>
+    <cellStyle name="Comma 2 2" xfId="11"/>
+    <cellStyle name="Comma 2 2 2" xfId="43"/>
+    <cellStyle name="Comma 2 2 3" xfId="44"/>
+    <cellStyle name="Comma 2 3" xfId="45"/>
+    <cellStyle name="Comma 3" xfId="46"/>
+    <cellStyle name="Comma 4" xfId="47"/>
+    <cellStyle name="Comma 5" xfId="48"/>
+    <cellStyle name="Comma 6" xfId="49"/>
+    <cellStyle name="Comma 7" xfId="50"/>
+    <cellStyle name="Currency 2" xfId="51"/>
+    <cellStyle name="Currency 3" xfId="52"/>
+    <cellStyle name="Currency 3 2" xfId="53"/>
+    <cellStyle name="Data" xfId="54"/>
+    <cellStyle name="Data no deci" xfId="55"/>
+    <cellStyle name="Data Superscript" xfId="56"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="57"/>
+    <cellStyle name="Explanatory Text 2" xfId="58"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Footnotes: top row" xfId="2"/>
+    <cellStyle name="Good 2" xfId="59"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
+    <cellStyle name="Heading 1 2" xfId="60"/>
+    <cellStyle name="Heading 2 2" xfId="61"/>
+    <cellStyle name="Heading 3 2" xfId="62"/>
+    <cellStyle name="Heading 4 2" xfId="63"/>
+    <cellStyle name="Hed Side" xfId="13"/>
+    <cellStyle name="Hed Side bold" xfId="64"/>
+    <cellStyle name="Hed Side Indent" xfId="65"/>
+    <cellStyle name="Hed Side Regular" xfId="66"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="67"/>
+    <cellStyle name="Hed Top" xfId="68"/>
     <cellStyle name="Hyperlink" xfId="140" builtinId="8"/>
-    <cellStyle name="Input 2" xfId="69" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Neutral 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Input 2" xfId="69"/>
+    <cellStyle name="Linked Cell 2" xfId="70"/>
+    <cellStyle name="Neutral 2" xfId="71"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="72" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Normal 11" xfId="10" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Normal 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Normal 2 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 2 3" xfId="76" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 2 4" xfId="77" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 3 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="79" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="80" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="81" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 3 3" xfId="82" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 3 4" xfId="86" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 3 5" xfId="88" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 3 6" xfId="89" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 3 7" xfId="90" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 3 8" xfId="91" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 3 9" xfId="12" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 4" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 4 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 4 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 4 2 3" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 4 3" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 4 3 3" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 4 4" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 4 4 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 4 5" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 4 6" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 4 7" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 4 8" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 5" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 5 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 5 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 6" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 7" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 8" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 9" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Note 2" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Note 2 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Output 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Percent 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Percent 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Percent 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Percent 3 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Source Hed" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Source Superscript" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Source Text" xfId="9" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="State" xfId="124" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Superscript" xfId="125" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Table Data" xfId="126" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Table Head Top" xfId="127" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Table Hed Side" xfId="128" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Title 2" xfId="129" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Title Text" xfId="130" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Title Text 1" xfId="131" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Title Text 2" xfId="132" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Title-1" xfId="14" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Title-2" xfId="133" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Title-3" xfId="134" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Total 2" xfId="135" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Warning Text 2" xfId="136" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Wrap" xfId="137" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Wrap Bold" xfId="138" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Wrap Title" xfId="139" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 10" xfId="72"/>
+    <cellStyle name="Normal 11" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="73"/>
+    <cellStyle name="Normal 2 2 2" xfId="74"/>
+    <cellStyle name="Normal 2 2 3" xfId="75"/>
+    <cellStyle name="Normal 2 3" xfId="76"/>
+    <cellStyle name="Normal 2 4" xfId="77"/>
+    <cellStyle name="Normal 3" xfId="8"/>
+    <cellStyle name="Normal 3 2" xfId="78"/>
+    <cellStyle name="Normal 3 2 2" xfId="79"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="80"/>
+    <cellStyle name="Normal 3 2 3" xfId="81"/>
+    <cellStyle name="Normal 3 3" xfId="82"/>
+    <cellStyle name="Normal 3 3 2" xfId="83"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="84"/>
+    <cellStyle name="Normal 3 3 3" xfId="85"/>
+    <cellStyle name="Normal 3 4" xfId="86"/>
+    <cellStyle name="Normal 3 4 2" xfId="87"/>
+    <cellStyle name="Normal 3 5" xfId="88"/>
+    <cellStyle name="Normal 3 6" xfId="89"/>
+    <cellStyle name="Normal 3 7" xfId="90"/>
+    <cellStyle name="Normal 3 8" xfId="91"/>
+    <cellStyle name="Normal 3 9" xfId="12"/>
+    <cellStyle name="Normal 4" xfId="92"/>
+    <cellStyle name="Normal 4 2" xfId="93"/>
+    <cellStyle name="Normal 4 2 2" xfId="94"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="95"/>
+    <cellStyle name="Normal 4 2 3" xfId="96"/>
+    <cellStyle name="Normal 4 3" xfId="97"/>
+    <cellStyle name="Normal 4 3 2" xfId="98"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="99"/>
+    <cellStyle name="Normal 4 3 3" xfId="100"/>
+    <cellStyle name="Normal 4 4" xfId="101"/>
+    <cellStyle name="Normal 4 4 2" xfId="102"/>
+    <cellStyle name="Normal 4 5" xfId="103"/>
+    <cellStyle name="Normal 4 6" xfId="104"/>
+    <cellStyle name="Normal 4 7" xfId="105"/>
+    <cellStyle name="Normal 4 8" xfId="106"/>
+    <cellStyle name="Normal 5" xfId="107"/>
+    <cellStyle name="Normal 5 2" xfId="108"/>
+    <cellStyle name="Normal 5 3" xfId="109"/>
+    <cellStyle name="Normal 6" xfId="110"/>
+    <cellStyle name="Normal 6 2" xfId="111"/>
+    <cellStyle name="Normal 7" xfId="112"/>
+    <cellStyle name="Normal 8" xfId="113"/>
+    <cellStyle name="Normal 9" xfId="114"/>
+    <cellStyle name="Note 2" xfId="115"/>
+    <cellStyle name="Note 2 2" xfId="116"/>
+    <cellStyle name="Output 2" xfId="117"/>
+    <cellStyle name="Parent row" xfId="3"/>
+    <cellStyle name="Percent 2" xfId="118"/>
+    <cellStyle name="Percent 2 2" xfId="119"/>
+    <cellStyle name="Percent 3" xfId="120"/>
+    <cellStyle name="Percent 3 2" xfId="121"/>
+    <cellStyle name="Source Hed" xfId="122"/>
+    <cellStyle name="Source Superscript" xfId="123"/>
+    <cellStyle name="Source Text" xfId="9"/>
+    <cellStyle name="State" xfId="124"/>
+    <cellStyle name="Superscript" xfId="125"/>
+    <cellStyle name="Table Data" xfId="126"/>
+    <cellStyle name="Table Head Top" xfId="127"/>
+    <cellStyle name="Table Hed Side" xfId="128"/>
+    <cellStyle name="Table title" xfId="7"/>
+    <cellStyle name="Title 2" xfId="129"/>
+    <cellStyle name="Title Text" xfId="130"/>
+    <cellStyle name="Title Text 1" xfId="131"/>
+    <cellStyle name="Title Text 2" xfId="132"/>
+    <cellStyle name="Title-1" xfId="14"/>
+    <cellStyle name="Title-2" xfId="133"/>
+    <cellStyle name="Title-3" xfId="134"/>
+    <cellStyle name="Total 2" xfId="135"/>
+    <cellStyle name="Warning Text 2" xfId="136"/>
+    <cellStyle name="Wrap" xfId="137"/>
+    <cellStyle name="Wrap Bold" xfId="138"/>
+    <cellStyle name="Wrap Title" xfId="139"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1623,23 +1623,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1675,23 +1658,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1867,14 +1833,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="2" max="2" width="73.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2202,15 +2168,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{F7E7A3DE-93B2-4E97-8034-BE9FA2CBB032}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{0A5F8456-85E2-4B46-98CB-42301965587F}"/>
-    <hyperlink ref="B28" r:id="rId3" display="https://www.icao.int/MID/Documents/2017/Aviation Data and Analysis Seminar/PPT3 - Airlines Operating costs and productivity.pdf" xr:uid="{32C07062-31D6-4D64-9941-54355C398A54}"/>
-    <hyperlink ref="B21" r:id="rId4" xr:uid="{A1682FDD-C2BD-495E-8A6B-5F03193720A5}"/>
-    <hyperlink ref="B35" r:id="rId5" xr:uid="{86CB5594-D53D-4996-A0D1-BB39C7D7D625}"/>
-    <hyperlink ref="B41" r:id="rId6" xr:uid="{B0ED8C7C-30CE-4966-BD3F-14CBF2AB2A2B}"/>
-    <hyperlink ref="B48" r:id="rId7" xr:uid="{B27ABC8E-899E-48AC-8608-F37B2EDFED93}"/>
-    <hyperlink ref="B55" r:id="rId8" display="http://www.sparusa.com/Presentations/Presentation-Commercial Ship Life Cycle &amp; Required Freight Rate (RFR) Cost Model.pdf" xr:uid="{4BC70352-C238-4681-9474-B434C82A9EE6}"/>
-    <hyperlink ref="B62" r:id="rId9" xr:uid="{5439DEF3-45BA-42A3-B033-B27D7C2B3817}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B28" r:id="rId3" display="https://www.icao.int/MID/Documents/2017/Aviation Data and Analysis Seminar/PPT3 - Airlines Operating costs and productivity.pdf"/>
+    <hyperlink ref="B21" r:id="rId4"/>
+    <hyperlink ref="B35" r:id="rId5"/>
+    <hyperlink ref="B41" r:id="rId6"/>
+    <hyperlink ref="B48" r:id="rId7"/>
+    <hyperlink ref="B55" r:id="rId8" display="http://www.sparusa.com/Presentations/Presentation-Commercial Ship Life Cycle &amp; Required Freight Rate (RFR) Cost Model.pdf"/>
+    <hyperlink ref="B62" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -2218,16 +2184,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA56E7A-E0B4-48E9-AA66-C39B91D43ABA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.59765625" customWidth="1"/>
+    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2891,13 +2859,13 @@
       <c r="A88" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="20">
-        <f>B54</f>
-        <v>3332119.6733545554</v>
-      </c>
-      <c r="C88" s="20">
-        <f>B55</f>
-        <v>2434118.0622207024</v>
+      <c r="B88" s="28">
+        <f>B54/10</f>
+        <v>333211.96733545553</v>
+      </c>
+      <c r="C88" s="28">
+        <f>B55/10</f>
+        <v>243411.80622207024</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2971,9 +2939,9 @@
       <c r="A96" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B96" s="20">
-        <f>B87</f>
-        <v>2279318.9754813975</v>
+      <c r="B96" s="28">
+        <f>B87/10</f>
+        <v>227931.89754813974</v>
       </c>
       <c r="C96" t="e">
         <f>NA()</f>
@@ -3021,9 +2989,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{DEA7D659-12AB-4A56-889B-D770D6477AD9}"/>
-    <hyperlink ref="B13" r:id="rId2" xr:uid="{83856772-5164-484D-9C39-5E905DAB68CE}"/>
-    <hyperlink ref="A65" r:id="rId3" xr:uid="{CF3217FC-13DF-41C0-A64F-4474765B54A2}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId2"/>
+    <hyperlink ref="A65" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -3031,22 +2999,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="8" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="8" width="23.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3178,31 +3148,31 @@
       </c>
       <c r="B5" s="5">
         <f>'Cost Data'!$C88</f>
-        <v>2434118.0622207024</v>
+        <v>243411.80622207024</v>
       </c>
       <c r="C5" s="5">
         <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <v>333211.96733545553</v>
       </c>
       <c r="D5" s="5">
         <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <v>333211.96733545553</v>
       </c>
       <c r="E5" s="5">
         <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <v>333211.96733545553</v>
       </c>
       <c r="F5" s="5">
         <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <v>333211.96733545553</v>
       </c>
       <c r="G5" s="5">
         <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <v>333211.96733545553</v>
       </c>
       <c r="H5" s="5">
         <f>'Cost Data'!$C88</f>
-        <v>2434118.0622207024</v>
+        <v>243411.80622207024</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3288,22 +3258,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="8" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="8" width="23.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3407,23 +3379,23 @@
       </c>
       <c r="C4" s="6">
         <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <v>227931.89754813974</v>
       </c>
       <c r="D4" s="6">
         <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <v>227931.89754813974</v>
       </c>
       <c r="E4" s="6">
         <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <v>227931.89754813974</v>
       </c>
       <c r="F4" s="6">
         <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <v>227931.89754813974</v>
       </c>
       <c r="G4" s="6">
         <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <v>227931.89754813974</v>
       </c>
       <c r="H4" s="26">
         <v>0</v>

</xml_diff>